<commit_message>
created first shift analysis Rmarkdown
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_child_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_child_subject_log.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC_NOVEL/bing_data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6F968349-89BD-FD49-B080-259BB545716F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="15620"/>
+    <workbookView xWindow="560" yWindow="900" windowWidth="25040" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="113">
   <si>
     <t>Subject ID</t>
   </si>
@@ -294,20 +300,86 @@
     <t xml:space="preserve">Leaned forward a lot </t>
   </si>
   <si>
+    <t>SAN-072618-01</t>
+  </si>
+  <si>
+    <t>SAN-072618-02</t>
+  </si>
+  <si>
+    <t>SAN-072618-03</t>
+  </si>
+  <si>
+    <t>SAN-072618-04</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Took off headphones right near beginning; asked me to come sit next to him near end, which didn't seem to be distracting</t>
+  </si>
+  <si>
+    <t>EI</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Leaned forward a lot; near end of word block 4, asked to go back to classroom</t>
+  </si>
+  <si>
+    <t>(maybe) drop word block 1</t>
+  </si>
+  <si>
     <t>order_key</t>
   </si>
   <si>
+    <t>nogaze_gaze_1_gr</t>
+  </si>
+  <si>
+    <t>nogaze_gaze_2_ol</t>
+  </si>
+  <si>
+    <t>gaze_nogaze_3_gr</t>
+  </si>
+  <si>
+    <t>gaze_nogaze_4_ol</t>
+  </si>
+  <si>
     <t>SAN-071218-04</t>
+  </si>
+  <si>
+    <t>SAN-073118-01</t>
+  </si>
+  <si>
+    <t>SAN-073118-02</t>
+  </si>
+  <si>
+    <t>SAN-073118-03</t>
+  </si>
+  <si>
+    <t>JO</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>Wore glasses but eye tracker seemed fine</t>
+  </si>
+  <si>
+    <t>Seemed tired at end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,6 +432,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -381,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -401,6 +480,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +542,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -513,7 +594,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -707,29 +788,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
     <col min="12" max="12" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +841,7 @@
         <v>36</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>10</v>
@@ -773,7 +856,7 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
@@ -802,7 +885,9 @@
       <c r="I2" s="14">
         <v>1</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="J2" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K2" s="14" t="s">
         <v>11</v>
       </c>
@@ -810,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
@@ -839,13 +924,15 @@
       <c r="I3" s="14">
         <v>1</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K3" s="14" t="s">
         <v>11</v>
       </c>
       <c r="L3" s="14"/>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
@@ -874,7 +961,9 @@
       <c r="I4" s="14">
         <v>1</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K4" s="14" t="s">
         <v>11</v>
       </c>
@@ -882,9 +971,9 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>24</v>
@@ -911,13 +1000,15 @@
       <c r="I5" s="14">
         <v>1</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="L5" s="14"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>22</v>
       </c>
@@ -946,7 +1037,9 @@
       <c r="I6" s="14">
         <v>1</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K6" s="14" t="s">
         <v>11</v>
       </c>
@@ -954,7 +1047,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>30</v>
       </c>
@@ -983,7 +1076,9 @@
       <c r="I7" s="14">
         <v>2</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K7" s="14" t="s">
         <v>38</v>
       </c>
@@ -991,7 +1086,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>31</v>
       </c>
@@ -1020,13 +1115,15 @@
       <c r="I8" s="14">
         <v>3</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>32</v>
       </c>
@@ -1055,13 +1152,15 @@
       <c r="I9" s="14">
         <v>4</v>
       </c>
-      <c r="J9" s="14"/>
+      <c r="J9" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K9" s="14"/>
       <c r="L9" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>33</v>
       </c>
@@ -1090,13 +1189,15 @@
       <c r="I10" s="14">
         <v>1</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K10" s="14"/>
       <c r="L10" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>47</v>
       </c>
@@ -1125,11 +1226,13 @@
       <c r="I11" s="14">
         <v>2</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>48</v>
       </c>
@@ -1158,13 +1261,15 @@
       <c r="I12" s="14">
         <v>3</v>
       </c>
-      <c r="J12" s="14"/>
+      <c r="J12" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="K12" s="14"/>
       <c r="L12" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
         <v>49</v>
       </c>
@@ -1193,7 +1298,9 @@
       <c r="I13" s="14">
         <v>4</v>
       </c>
-      <c r="J13" s="14"/>
+      <c r="J13" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K13" s="14" t="s">
         <v>86</v>
       </c>
@@ -1201,7 +1308,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>58</v>
       </c>
@@ -1230,11 +1337,13 @@
       <c r="I14" s="14">
         <v>1</v>
       </c>
-      <c r="J14" s="14"/>
+      <c r="J14" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K14" s="14"/>
       <c r="L14" s="14"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>59</v>
       </c>
@@ -1263,11 +1372,13 @@
       <c r="I15" s="14">
         <v>2</v>
       </c>
-      <c r="J15" s="14"/>
+      <c r="J15" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K15" s="14"/>
       <c r="L15" s="14"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>60</v>
       </c>
@@ -1296,11 +1407,13 @@
       <c r="I16" s="14">
         <v>3</v>
       </c>
-      <c r="J16" s="14"/>
+      <c r="J16" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>65</v>
       </c>
@@ -1329,7 +1442,9 @@
       <c r="I17" s="14">
         <v>4</v>
       </c>
-      <c r="J17" s="14"/>
+      <c r="J17" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K17" s="14" t="s">
         <v>38</v>
       </c>
@@ -1337,7 +1452,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>66</v>
       </c>
@@ -1366,7 +1481,9 @@
       <c r="I18" s="14">
         <v>4</v>
       </c>
-      <c r="J18" s="14"/>
+      <c r="J18" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K18" s="14" t="s">
         <v>38</v>
       </c>
@@ -1374,7 +1491,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -1403,11 +1520,13 @@
       <c r="I19" s="14">
         <v>4</v>
       </c>
-      <c r="J19" s="14"/>
+      <c r="J19" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K19" s="14"/>
       <c r="L19" s="14"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>68</v>
       </c>
@@ -1436,7 +1555,9 @@
       <c r="I20" s="14">
         <v>1</v>
       </c>
-      <c r="J20" s="14"/>
+      <c r="J20" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K20" s="14"/>
       <c r="L20" s="14" t="s">
         <v>73</v>
@@ -1448,7 +1569,7 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>74</v>
       </c>
@@ -1477,7 +1598,9 @@
       <c r="I21" s="14">
         <v>1</v>
       </c>
-      <c r="J21" s="14"/>
+      <c r="J21" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K21" s="14"/>
       <c r="L21" s="14" t="s">
         <v>80</v>
@@ -1489,7 +1612,7 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>75</v>
       </c>
@@ -1518,7 +1641,9 @@
       <c r="I22" s="14">
         <v>2</v>
       </c>
-      <c r="J22" s="14"/>
+      <c r="J22" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K22" s="14"/>
       <c r="L22" s="14" t="s">
         <v>79</v>
@@ -1530,7 +1655,7 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>81</v>
       </c>
@@ -1559,7 +1684,9 @@
       <c r="I23" s="14">
         <v>3</v>
       </c>
-      <c r="J23" s="14"/>
+      <c r="J23" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="K23" s="14"/>
       <c r="L23" s="14" t="s">
         <v>88</v>
@@ -1571,7 +1698,7 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>82</v>
       </c>
@@ -1600,7 +1727,9 @@
       <c r="I24" s="14">
         <v>4</v>
       </c>
-      <c r="J24" s="14"/>
+      <c r="J24" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K24" s="14" t="s">
         <v>87</v>
       </c>
@@ -1614,24 +1743,44 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" s="15">
+        <v>43307</v>
+      </c>
+      <c r="D25" s="15">
+        <v>42185</v>
+      </c>
       <c r="E25" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
+        <v>3.0722222222222224</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="H25" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
+      <c r="I25" s="14">
+        <v>1</v>
+      </c>
+      <c r="J25" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -1639,24 +1788,42 @@
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
     </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="15">
+        <v>43307</v>
+      </c>
+      <c r="D26" s="15">
+        <v>41752</v>
+      </c>
       <c r="E26" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
+        <v>4.2583333333333337</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="H26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+      <c r="I26" s="14">
+        <v>2</v>
+      </c>
+      <c r="J26" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
+      <c r="L26" s="14" t="s">
+        <v>98</v>
+      </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -1664,24 +1831,42 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
     </row>
-    <row r="27" spans="1:18">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="15">
+        <v>43307</v>
+      </c>
+      <c r="D27" s="15">
+        <v>41944</v>
+      </c>
       <c r="E27" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
+        <v>3.7361111111111112</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>72</v>
+      </c>
       <c r="H27" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="I27" s="14">
+        <v>3</v>
+      </c>
+      <c r="J27" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
+      <c r="L27" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -1689,22 +1874,38 @@
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
     </row>
-    <row r="28" spans="1:18">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="15">
+        <v>43307</v>
+      </c>
+      <c r="D28" s="15">
+        <v>41703</v>
+      </c>
       <c r="E28" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+        <v>4.3916666666666666</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="H28" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
+      <c r="I28" s="14">
+        <v>4</v>
+      </c>
+      <c r="J28" s="17" t="s">
+        <v>104</v>
+      </c>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
       <c r="M28" s="4"/>
@@ -1714,24 +1915,42 @@
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
     </row>
-    <row r="29" spans="1:18">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="15">
+        <v>43312</v>
+      </c>
+      <c r="D29" s="15">
+        <v>41515</v>
+      </c>
       <c r="E29" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+        <v>4.9222222222222225</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="H29" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="I29" s="14">
+        <v>1</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
+      <c r="L29" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -1739,24 +1958,42 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="15">
+        <v>43312</v>
+      </c>
+      <c r="D30" s="15">
+        <v>42046</v>
+      </c>
       <c r="E30" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
+        <v>3.4722222222222223</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>97</v>
+      </c>
       <c r="H30" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="I30" s="14">
+        <v>2</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
+      <c r="L30" s="14" t="s">
+        <v>112</v>
+      </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -1764,22 +2001,38 @@
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
     </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C31" s="15">
+        <v>43312</v>
+      </c>
+      <c r="D31" s="15">
+        <v>41871</v>
+      </c>
       <c r="E31" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+        <v>3.9472222222222224</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>71</v>
+      </c>
       <c r="H31" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
+      <c r="I31" s="14">
+        <v>3</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="K31" s="14"/>
       <c r="L31" s="14"/>
       <c r="M31" s="4"/>
@@ -1789,10 +2042,10 @@
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="8"/>
       <c r="E32" s="4">
         <f t="shared" si="0"/>
@@ -1811,7 +2064,7 @@
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
     </row>
-    <row r="33" spans="1:18">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -1835,7 +2088,7 @@
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
     </row>
-    <row r="34" spans="1:18">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7"/>
@@ -1856,7 +2109,7 @@
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
     </row>
-    <row r="35" spans="1:18">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1876,7 +2129,7 @@
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="C36" s="7"/>
@@ -1897,7 +2150,7 @@
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1921,7 +2174,7 @@
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
     </row>
-    <row r="38" spans="1:18">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="8"/>
@@ -1943,7 +2196,7 @@
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
@@ -1967,7 +2220,7 @@
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7"/>
@@ -1988,7 +2241,7 @@
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
     </row>
-    <row r="41" spans="1:18">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="C41" s="7"/>
@@ -2009,7 +2262,7 @@
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="C42" s="8"/>
@@ -2031,7 +2284,7 @@
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="8"/>
@@ -2053,7 +2306,7 @@
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="C44" s="8"/>
@@ -2075,7 +2328,7 @@
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="10"/>
@@ -2099,7 +2352,7 @@
       <c r="Q45" s="11"/>
       <c r="R45" s="11"/>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="12"/>
       <c r="C46" s="13"/>
@@ -2120,7 +2373,7 @@
       <c r="N46" s="12"/>
       <c r="O46" s="12"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="13"/>
@@ -2135,7 +2388,7 @@
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
     </row>
-    <row r="48" spans="1:18">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
@@ -2150,7 +2403,7 @@
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
@@ -2165,7 +2418,7 @@
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
       <c r="B50" s="12"/>
       <c r="C50" s="13"/>
@@ -2180,7 +2433,7 @@
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="13"/>
@@ -2195,7 +2448,7 @@
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="12"/>
       <c r="B52" s="12"/>
       <c r="C52" s="13"/>
@@ -2210,7 +2463,7 @@
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="12"/>
       <c r="B53" s="12"/>
       <c r="C53" s="13"/>
@@ -2225,7 +2478,7 @@
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="12"/>
       <c r="B54" s="12"/>
       <c r="C54" s="7"/>
@@ -2240,7 +2493,7 @@
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B55" s="12"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
@@ -2252,7 +2505,7 @@
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B56" s="12"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -2264,7 +2517,7 @@
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B57" s="12"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
@@ -2276,7 +2529,7 @@
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B58" s="12"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -2288,7 +2541,7 @@
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B59" s="12"/>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
@@ -2300,7 +2553,7 @@
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B60" s="12"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
@@ -2312,7 +2565,7 @@
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B61" s="12"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
@@ -2324,7 +2577,7 @@
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B62" s="12"/>
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
@@ -2336,7 +2589,7 @@
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B63" s="12"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
@@ -2348,7 +2601,7 @@
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B64" s="12"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
@@ -2360,7 +2613,7 @@
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
     </row>
-    <row r="65" spans="2:10">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B65" s="12"/>
       <c r="C65" s="7"/>
       <c r="D65" s="7"/>
@@ -2372,7 +2625,7 @@
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
     </row>
-    <row r="66" spans="2:10">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66" s="12"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
@@ -2384,7 +2637,7 @@
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
     </row>
-    <row r="67" spans="2:10">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B67" s="12"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
@@ -2396,7 +2649,7 @@
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
     </row>
-    <row r="68" spans="2:10">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B68" s="12"/>
       <c r="C68" s="7"/>
       <c r="D68" s="7"/>
@@ -2408,7 +2661,7 @@
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
     </row>
-    <row r="69" spans="2:10">
+    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B69" s="12"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
@@ -2420,7 +2673,7 @@
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
     </row>
-    <row r="70" spans="2:10">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B70" s="12"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
@@ -2432,7 +2685,7 @@
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
     </row>
-    <row r="71" spans="2:10">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B71" s="12"/>
       <c r="C71" s="7"/>
       <c r="D71" s="7"/>
@@ -2444,7 +2697,7 @@
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
     </row>
-    <row r="72" spans="2:10">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B72" s="12"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
@@ -2456,7 +2709,7 @@
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
     </row>
-    <row r="73" spans="2:10">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="4">
@@ -2467,7 +2720,7 @@
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
     </row>
-    <row r="74" spans="2:10">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="4">
@@ -2478,7 +2731,7 @@
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
     </row>
-    <row r="75" spans="2:10">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="4">
@@ -2489,7 +2742,7 @@
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
     </row>
-    <row r="76" spans="2:10">
+    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="4">
@@ -2500,7 +2753,7 @@
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
     </row>
-    <row r="77" spans="2:10">
+    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C77" s="7"/>
       <c r="D77" s="7"/>
       <c r="E77" s="4">
@@ -2511,7 +2764,7 @@
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
     </row>
-    <row r="78" spans="2:10">
+    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C78" s="7"/>
       <c r="D78" s="7"/>
       <c r="E78" s="4">
@@ -2522,7 +2775,7 @@
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
     </row>
-    <row r="79" spans="2:10">
+    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="4">
@@ -2533,7 +2786,7 @@
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
     </row>
-    <row r="80" spans="2:10">
+    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
       <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="4">
@@ -2544,7 +2797,7 @@
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
     </row>
-    <row r="81" spans="3:10">
+    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
       <c r="E81" s="4">
@@ -2555,7 +2808,7 @@
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
     </row>
-    <row r="82" spans="3:10">
+    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C82" s="7"/>
       <c r="D82" s="7"/>
       <c r="E82" s="4">
@@ -2566,7 +2819,7 @@
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
     </row>
-    <row r="83" spans="3:10">
+    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="4">
@@ -2577,7 +2830,7 @@
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
     </row>
-    <row r="84" spans="3:10">
+    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C84" s="7"/>
       <c r="D84" s="7"/>
       <c r="E84" s="4">
@@ -2588,7 +2841,7 @@
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
     </row>
-    <row r="85" spans="3:10">
+    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="4">
@@ -2599,7 +2852,7 @@
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
     </row>
-    <row r="86" spans="3:10">
+    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C86" s="7"/>
       <c r="D86" s="7"/>
       <c r="E86" s="4">
@@ -2610,7 +2863,7 @@
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
     </row>
-    <row r="87" spans="3:10">
+    <row r="87" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="4">
@@ -2621,67 +2874,67 @@
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
     </row>
-    <row r="88" spans="3:10">
+    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E88" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="3:10">
+    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E89" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="3:10">
+    <row r="90" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E90" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="3:10">
+    <row r="91" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E91" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:10">
+    <row r="92" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E92" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="3:10">
+    <row r="93" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E93" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="3:10">
+    <row r="94" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E94" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="3:10">
+    <row r="95" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E95" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="3:10">
+    <row r="96" spans="3:10" x14ac:dyDescent="0.2">
       <c r="E96" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="5:5">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E97" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="5:5">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E98" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2689,10 +2942,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated child and adult subject logs
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_child_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_child_subject_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C11CE5-4A72-E141-BC3B-28F645DCB11C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBC0681-6251-B24C-8B67-1BD050561106}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="900" windowWidth="25040" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="114">
   <si>
     <t>ES</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Seemed tired at end</t>
   </si>
   <si>
-    <t>sub_id</t>
-  </si>
-  <si>
     <t>child_initials</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>ethnicity/race</t>
-  </si>
-  <si>
     <t>experimenter</t>
   </si>
   <si>
@@ -370,6 +364,15 @@
   </si>
   <si>
     <t>Took off headphones right near beginning (trial 0 of 1st word block); asked me to come sit next to him near end, which didn't seem to be distracting</t>
+  </si>
+  <si>
+    <t>subid</t>
+  </si>
+  <si>
+    <t>ethnicity_race</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -796,7 +799,7 @@
   <dimension ref="A1:R98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,55 +807,56 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
     <col min="13" max="13" width="14.1640625" customWidth="1"/>
     <col min="14" max="14" width="145.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>93</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="J1" s="15" t="s">
         <v>78</v>
       </c>
       <c r="K1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>99</v>
       </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
@@ -888,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>26</v>
@@ -896,7 +900,9 @@
       <c r="L2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="12"/>
+      <c r="M2" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N2" s="12" t="s">
         <v>2</v>
       </c>
@@ -930,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="J3" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K3" s="12" t="s">
         <v>26</v>
@@ -938,7 +944,9 @@
       <c r="L3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N3" s="12"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
@@ -961,7 +969,7 @@
         <v>7</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>0</v>
@@ -970,7 +978,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K4" s="12" t="s">
         <v>26</v>
@@ -978,7 +986,9 @@
       <c r="L4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="12"/>
+      <c r="M4" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N4" s="12" t="s">
         <v>17</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K5" s="12" t="s">
         <v>26</v>
@@ -1020,7 +1030,9 @@
       <c r="L5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M5" s="12"/>
+      <c r="M5" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
@@ -1052,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>26</v>
@@ -1060,7 +1072,9 @@
       <c r="L6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="12"/>
+      <c r="M6" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N6" s="12" t="s">
         <v>18</v>
       </c>
@@ -1094,15 +1108,19 @@
         <v>2</v>
       </c>
       <c r="J7" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
@@ -1134,13 +1152,17 @@
         <v>3</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K8" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N8" s="12" t="s">
         <v>33</v>
       </c>
@@ -1174,12 +1196,17 @@
         <v>4</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="M9" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N9" s="12" t="s">
         <v>32</v>
       </c>
@@ -1213,13 +1240,17 @@
         <v>1</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N10" s="12" t="s">
         <v>29</v>
       </c>
@@ -1244,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>0</v>
@@ -1253,13 +1284,17 @@
         <v>2</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L11" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
@@ -1282,7 +1317,7 @@
         <v>7</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>0</v>
@@ -1291,13 +1326,17 @@
         <v>3</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N12" s="12" t="s">
         <v>41</v>
       </c>
@@ -1331,17 +1370,19 @@
         <v>4</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L13" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="M13" s="12">
         <v>4</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -1373,13 +1414,17 @@
         <v>1</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -1411,13 +1456,17 @@
         <v>2</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M15" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
@@ -1449,13 +1498,17 @@
         <v>3</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
@@ -1478,7 +1531,7 @@
         <v>7</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>0</v>
@@ -1487,13 +1540,17 @@
         <v>4</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L17" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N17" s="12" t="s">
         <v>17</v>
       </c>
@@ -1527,13 +1584,17 @@
         <v>4</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K18" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N18" s="12" t="s">
         <v>17</v>
       </c>
@@ -1567,13 +1628,17 @@
         <v>4</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
@@ -1605,13 +1670,17 @@
         <v>1</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K20" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L20" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M20" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N20" s="12" t="s">
         <v>57</v>
       </c>
@@ -1649,13 +1718,17 @@
         <v>1</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M21" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N21" s="12" t="s">
         <v>64</v>
       </c>
@@ -1693,13 +1766,17 @@
         <v>2</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M22" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N22" s="12" t="s">
         <v>63</v>
       </c>
@@ -1737,15 +1814,19 @@
         <v>3</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K23" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M23" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N23" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -1781,17 +1862,19 @@
         <v>4</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K24" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L24" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L24" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="M24" s="12">
         <v>2</v>
       </c>
       <c r="N24" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -1827,15 +1910,19 @@
         <v>1</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N25" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
@@ -1871,13 +1958,17 @@
         <v>2</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M26" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N26" s="12" t="s">
         <v>77</v>
       </c>
@@ -1915,15 +2006,19 @@
         <v>3</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M27" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N27" s="12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
@@ -1959,13 +2054,17 @@
         <v>4</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N28" s="12"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -2001,13 +2100,17 @@
         <v>1</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L29" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M29" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N29" s="12" t="s">
         <v>85</v>
       </c>
@@ -2045,13 +2148,17 @@
         <v>2</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K30" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L30" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N30" s="12" t="s">
         <v>86</v>
       </c>
@@ -2089,13 +2196,17 @@
         <v>3</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="N31" s="12"/>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
@@ -2108,7 +2219,7 @@
       <c r="C32" s="14"/>
       <c r="D32" s="6"/>
       <c r="E32" s="2">
-        <f t="shared" ref="E5:E68" si="0">YEARFRAC(D32,C32)</f>
+        <f t="shared" ref="E32:E68" si="0">YEARFRAC(D32,C32)</f>
         <v>0</v>
       </c>
       <c r="F32" s="4"/>

</xml_diff>

<commit_message>
updated child subject log 8/9/18
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_child_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_child_subject_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DEA3D5E-A6F4-254D-9CF9-4201552A5201}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9F3E02-3C85-F040-97E6-99BDA2D2598B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="157">
   <si>
     <t>ES</t>
   </si>
@@ -394,6 +394,114 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>SAN-080718-01</t>
+  </si>
+  <si>
+    <t>JOR</t>
+  </si>
+  <si>
+    <t>SAN-080718-02</t>
+  </si>
+  <si>
+    <t>JY</t>
+  </si>
+  <si>
+    <t>SAN-080718-03</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>SAN-080718-04</t>
+  </si>
+  <si>
+    <t>AH</t>
+  </si>
+  <si>
+    <t>C </t>
+  </si>
+  <si>
+    <t>SAN-080718-05</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>C, ME</t>
+  </si>
+  <si>
+    <t>SAN-080918-01</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>A, C</t>
+  </si>
+  <si>
+    <t>SAN-080918-02</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>SAN-080918-03</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>no data collected</t>
+  </si>
+  <si>
+    <t>SAN-080918-04</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>SAN-080918-05</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>SAN-080918-06</t>
+  </si>
+  <si>
+    <t>SAN-080918-07</t>
+  </si>
+  <si>
+    <t>SAN-080918-08</t>
+  </si>
+  <si>
+    <t>ND</t>
+  </si>
+  <si>
+    <t>Mej</t>
+  </si>
+  <si>
+    <t>SAN-080918-09</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>SAN-080918-10</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>A, H/</t>
+  </si>
+  <si>
+    <t>SAN-080918-11</t>
+  </si>
+  <si>
+    <t>HR</t>
   </si>
 </sst>
 </file>
@@ -815,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2286,24 +2394,48 @@
       <c r="T31" s="2"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+      <c r="A32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="9">
+        <v>43319</v>
+      </c>
+      <c r="D32" s="9">
+        <v>41822</v>
+      </c>
       <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+        <v>4.0972222220000001</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="I32" s="2">
+        <v>4</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="O32" s="8" t="s">
         <v>97</v>
       </c>
@@ -2316,23 +2448,45 @@
       <c r="T32" s="2"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33">
-        <v>0</v>
-      </c>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="A33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="9">
+        <v>43319</v>
+      </c>
+      <c r="D33" s="9">
+        <v>41263</v>
+      </c>
+      <c r="E33" s="2">
+        <v>5.630555556</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H33" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I33" s="2"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="I33" s="2">
+        <v>1</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" s="8" t="s">
         <v>97</v>
@@ -2344,23 +2498,45 @@
       <c r="T33" s="2"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
+      <c r="A34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="9">
+        <v>43319</v>
+      </c>
+      <c r="D34" s="9">
+        <v>41804</v>
+      </c>
       <c r="E34" s="2">
-        <v>0</v>
-      </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+        <v>4.1472222219999999</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H34" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I34" s="2"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
+      <c r="I34" s="2">
+        <v>2</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N34" s="2"/>
       <c r="O34" s="8" t="s">
         <v>97</v>
@@ -2372,23 +2548,45 @@
       <c r="T34" s="2"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="A35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="9">
+        <v>43319</v>
+      </c>
+      <c r="D35" s="9">
+        <v>42097</v>
+      </c>
       <c r="E35" s="2">
-        <v>0</v>
-      </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+        <v>3.3444444440000001</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="H35" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I35" s="2"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="I35" s="2">
+        <v>3</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N35" s="2"/>
       <c r="O35" s="8" t="s">
         <v>97</v>
@@ -2400,24 +2598,48 @@
       <c r="T35" s="2"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36">
-        <v>0</v>
-      </c>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="A36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="9">
+        <v>43319</v>
+      </c>
+      <c r="D36" s="9">
+        <v>41173</v>
+      </c>
+      <c r="E36" s="2">
+        <v>5.8777777779999996</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="H36" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="I36" s="2">
+        <v>4</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="O36" s="8" t="s">
         <v>97</v>
       </c>
@@ -2430,23 +2652,45 @@
       <c r="T36" s="2"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
+      <c r="A37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D37" s="9">
+        <v>41547</v>
+      </c>
       <c r="E37" s="2">
-        <v>0</v>
-      </c>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+        <v>4.858333333</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="H37" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
+      <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N37" s="2"/>
       <c r="O37" s="8" t="s">
         <v>97</v>
@@ -2458,24 +2702,48 @@
       <c r="T37" s="2"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
+      <c r="A38" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D38" s="9">
+        <v>41821</v>
+      </c>
       <c r="E38" s="2">
-        <v>0</v>
-      </c>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+        <v>4.1055555559999997</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H38" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I38" s="2"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
+      <c r="I38" s="2">
+        <v>2</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="O38" s="8" t="s">
         <v>97</v>
       </c>
@@ -2488,23 +2756,45 @@
       <c r="T38" s="2"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39">
-        <v>0</v>
-      </c>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D39" s="9">
+        <v>41525</v>
+      </c>
+      <c r="E39" s="2">
+        <v>4.9194444439999998</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H39" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
+      <c r="I39" s="2">
+        <v>3</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N39" s="2"/>
       <c r="O39" s="8" t="s">
         <v>97</v>
@@ -2516,24 +2806,46 @@
       <c r="T39" s="2"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
+      <c r="A40" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D40" s="9">
+        <v>42010</v>
+      </c>
       <c r="E40" s="2">
-        <v>0</v>
-      </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+        <v>3.5916666670000001</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H40" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I40" s="2"/>
+      <c r="I40" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="K40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="O40" s="8" t="s">
         <v>97</v>
       </c>
@@ -2546,23 +2858,45 @@
       <c r="T40" s="2"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
+      <c r="A41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D41" s="9">
+        <v>41416</v>
+      </c>
       <c r="E41" s="2">
-        <v>0</v>
-      </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+        <v>5.2138888889999997</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="H41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
+      <c r="I41" s="2">
+        <v>4</v>
+      </c>
+      <c r="J41" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N41" s="2"/>
       <c r="O41" s="8" t="s">
         <v>97</v>
@@ -2574,24 +2908,48 @@
       <c r="T41" s="2"/>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="A42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D42" s="9">
+        <v>42183</v>
+      </c>
+      <c r="E42" s="2">
+        <v>3.113888889</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
+      <c r="I42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="O42" s="8" t="s">
         <v>97</v>
       </c>
@@ -2604,24 +2962,48 @@
       <c r="T42" s="2"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="A43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D43" s="9">
+        <v>41768</v>
+      </c>
       <c r="E43" s="2">
-        <v>0</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+        <v>4.25</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="H43" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
+      <c r="I43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="O43" s="8" t="s">
         <v>97</v>
       </c>
@@ -2634,23 +3016,45 @@
       <c r="T43" s="2"/>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
+      <c r="A44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D44" s="9">
+        <v>41985</v>
+      </c>
       <c r="E44" s="2">
-        <v>0</v>
-      </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+        <v>3.6583333329999999</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>149</v>
+      </c>
       <c r="H44" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I44" s="2"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
+      <c r="I44" s="2">
+        <v>1</v>
+      </c>
+      <c r="J44" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" s="8" t="s">
         <v>97</v>
@@ -2662,23 +3066,45 @@
       <c r="T44" s="2"/>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="A45" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D45" s="9">
+        <v>42031</v>
+      </c>
+      <c r="E45" s="2">
+        <v>3.5333333329999999</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="H45" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I45" s="2"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
+      <c r="I45" s="2">
+        <v>2</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" s="8" t="s">
         <v>97</v>
@@ -2690,23 +3116,45 @@
       <c r="T45" s="5"/>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
+      <c r="A46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D46" s="9">
+        <v>41988</v>
+      </c>
       <c r="E46" s="2">
-        <v>0</v>
-      </c>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+        <v>3.65</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="H46" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
+      <c r="I46" s="2">
+        <v>3</v>
+      </c>
+      <c r="J46" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N46" s="2"/>
       <c r="O46" s="8" t="s">
         <v>97</v>
@@ -2715,24 +3163,48 @@
       <c r="Q46" s="6"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
+      <c r="A47" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="9">
+        <v>43321</v>
+      </c>
+      <c r="D47" s="9">
+        <v>41279</v>
+      </c>
       <c r="E47" s="2">
-        <v>0</v>
-      </c>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+        <v>5.5944444439999996</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I47" s="2"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="I47" s="2">
+        <v>4</v>
+      </c>
+      <c r="J47" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M47" s="2">
+        <v>4</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="O47" s="8">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
fixed mistake in child subject log (needed to add NAs)
</commit_message>
<xml_diff>
--- a/data/01_participant_logs/elizabeth_child_subject_log.xlsx
+++ b/data/01_participant_logs/elizabeth_child_subject_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethswanson/Documents/speed-acc-novel/data/01_participant_logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD9F3E02-3C85-F040-97E6-99BDA2D2598B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3939EC7-D5FD-6A47-9A36-EE5D517CC5FF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="157">
   <si>
     <t>ES</t>
   </si>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2790,7 +2790,7 @@
         <v>96</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>97</v>
@@ -2833,7 +2833,9 @@
       <c r="I40" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J40" s="2"/>
+      <c r="J40" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="K40" s="2" t="s">
         <v>27</v>
       </c>
@@ -2942,7 +2944,7 @@
         <v>27</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>97</v>

</xml_diff>